<commit_message>
Refactored TestDataGenerator to read files, optimized summary map, tests for TestDataGenerator within Spring context
</commit_message>
<xml_diff>
--- a/src/test/resources/sheet.xlsx
+++ b/src/test/resources/sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>BoA-7797</t>
   </si>
@@ -28,7 +28,46 @@
     <t>EDISON WATER UTILITY Bill Payment</t>
   </si>
   <si>
-    <t>153 Orange</t>
+    <t>City of Philadelphia Bill Payment</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>332 Robbins</t>
+  </si>
+  <si>
+    <t>ZelleTony for Beacon clean sewer pipe etc.</t>
+  </si>
+  <si>
+    <t>Repairs</t>
+  </si>
+  <si>
+    <t>207 Beacon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steven </t>
+  </si>
+  <si>
+    <t>Cleaning &amp; maintenance</t>
+  </si>
+  <si>
+    <t>BoA-8211</t>
+  </si>
+  <si>
+    <t>RAPIN FRITURA RESTAURANT NEWARK NJ</t>
+  </si>
+  <si>
+    <t>Meal - C</t>
+  </si>
+  <si>
+    <t>OPTIMUM 7875 973-230-6046 NY</t>
+  </si>
+  <si>
+    <t>Phone/Cable/Internet</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -77,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -104,6 +143,15 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -341,7 +389,7 @@
         <v>113.0</v>
       </c>
       <c r="F1" s="5">
-        <f t="shared" ref="F1:F2" si="1">if(And(G1&lt;&gt;"",H1&lt;&gt;""),if(E1&lt;&gt;"",E1,D1),)</f>
+        <f t="shared" ref="F1:F7" si="1">if(And(G1&lt;&gt;"",H1&lt;&gt;""),if(E1&lt;&gt;"",E1,D1),)</f>
         <v>113</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -375,19 +423,169 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
+      <c r="H2" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44635.0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>737.0</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8">
+        <f t="shared" si="1"/>
+        <v>737</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44706.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3500.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2200.0</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44706.0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3500.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>480.0</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44662.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3">
+        <v>58.45</v>
+      </c>
+      <c r="E6" s="4">
+        <v>29.23</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="1"/>
+        <v>29.23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44858.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3">
+        <v>50.65</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8">
+        <f t="shared" si="1"/>
+        <v>50.65</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="H1:H2">
+    <dataValidation type="list" allowBlank="1" sqref="H1:H7">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G1:G2">
+    <dataValidation type="list" allowBlank="1" sqref="G1:G7">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Jira 66 refactor rdp repo methods (#11)
* Refactored TestDataGenerator to read files, optimized summary map, tests for TestDataGenerator within Spring context

* BizService tests out of spring context, working with InjectMocks/Mockito etc

* all tests out of Spring context using Mockito

* JPA tests working, full mvn clean test works

* implement unit tests for bizreportservice, fileprocessorservice
</commit_message>
<xml_diff>
--- a/src/test/resources/sheet.xlsx
+++ b/src/test/resources/sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>BoA-7797</t>
   </si>
@@ -28,7 +28,46 @@
     <t>EDISON WATER UTILITY Bill Payment</t>
   </si>
   <si>
-    <t>153 Orange</t>
+    <t>City of Philadelphia Bill Payment</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>332 Robbins</t>
+  </si>
+  <si>
+    <t>ZelleTony for Beacon clean sewer pipe etc.</t>
+  </si>
+  <si>
+    <t>Repairs</t>
+  </si>
+  <si>
+    <t>207 Beacon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steven </t>
+  </si>
+  <si>
+    <t>Cleaning &amp; maintenance</t>
+  </si>
+  <si>
+    <t>BoA-8211</t>
+  </si>
+  <si>
+    <t>RAPIN FRITURA RESTAURANT NEWARK NJ</t>
+  </si>
+  <si>
+    <t>Meal - C</t>
+  </si>
+  <si>
+    <t>OPTIMUM 7875 973-230-6046 NY</t>
+  </si>
+  <si>
+    <t>Phone/Cable/Internet</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -77,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -104,6 +143,15 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -341,7 +389,7 @@
         <v>113.0</v>
       </c>
       <c r="F1" s="5">
-        <f t="shared" ref="F1:F2" si="1">if(And(G1&lt;&gt;"",H1&lt;&gt;""),if(E1&lt;&gt;"",E1,D1),)</f>
+        <f t="shared" ref="F1:F7" si="1">if(And(G1&lt;&gt;"",H1&lt;&gt;""),if(E1&lt;&gt;"",E1,D1),)</f>
         <v>113</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -375,19 +423,169 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
+      <c r="H2" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44635.0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>737.0</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8">
+        <f t="shared" si="1"/>
+        <v>737</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44706.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3500.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2200.0</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44706.0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3500.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>480.0</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44662.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3">
+        <v>58.45</v>
+      </c>
+      <c r="E6" s="4">
+        <v>29.23</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="1"/>
+        <v>29.23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44858.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3">
+        <v>50.65</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8">
+        <f t="shared" si="1"/>
+        <v>50.65</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="H1:H2">
+    <dataValidation type="list" allowBlank="1" sqref="H1:H7">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G1:G2">
+    <dataValidation type="list" allowBlank="1" sqref="G1:G7">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>